<commit_message>
optmize logic -> uml reflection relationship and orgnization
Change-Id: I8112fa687e2d108e0ca22d599d753282a4cd7cee
</commit_message>
<xml_diff>
--- a/uml/android_source_learning_arg_table.xlsx
+++ b/uml/android_source_learning_arg_table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heavy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heavy/workspace/git-space/open/android/AndroidUmls/uml/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="700" windowWidth="30080" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="5240" yWindow="540" windowWidth="30080" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="system_core" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="24">
   <si>
     <t>方法(函数)</t>
     <rPh sb="0" eb="1">
@@ -184,6 +184,35 @@
     <rPh sb="31" eb="32">
       <t>fu'wu</t>
     </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>framework/base/cmd/app_process/app_main.cpp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>className</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>zygote执行时置空</t>
+    <rPh sb="6" eb="7">
+      <t>zhi'xing</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>shi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>zhi'kong</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>app_start</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -568,31 +597,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="6" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" style="4" customWidth="1"/>
-    <col min="4" max="5" width="10.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="78.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="33.33203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="26.6640625" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="4"/>
+    <col min="4" max="4" width="10.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="78.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="33.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -602,30 +631,27 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="I1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
@@ -634,22 +660,65 @@
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>